<commit_message>
Make trivia question text better and fix small loader bugs
</commit_message>
<xml_diff>
--- a/Data/Trivia Questions.xlsx
+++ b/Data/Trivia Questions.xlsx
@@ -24,89 +24,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
-  <si>
-    <t>Solar power generates electricity from what source?</t>
-  </si>
-  <si>
-    <t>Did the Apple iPhone first become available in 2005, 2006 or 2007?</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="94">
   <si>
     <t>In terms of computing, what does CPU stand for?</t>
   </si>
   <si>
-    <t>True or false? Nintendo was founded after the year 1900.</t>
-  </si>
-  <si>
     <t>The Hubble Space Telescope is named after which American astronomer?</t>
   </si>
   <si>
-    <t>Is the wavelength of infrared light too long or short to be seen by humans?</t>
-  </si>
-  <si>
-    <t>Firefox, Opera, Chrome, Safari and Explorer are types of what?</t>
-  </si>
-  <si>
-    <t>True or false? Gold is not a good conductor of electricity?</t>
-  </si>
-  <si>
     <t>The technologically advanced humanoid robot ASIMO is made by which car company?</t>
   </si>
   <si>
-    <t>True or false? Atomic bombs work by atomic fission.</t>
-  </si>
-  <si>
     <t>In terms of computing, what does ROM stand for?</t>
   </si>
   <si>
-    <t>Did the original Sony Playstation use CDs or cartridges to play games?</t>
-  </si>
-  <si>
-    <t>IBM is a well known computer and information technology company, what does IBM stand for?</t>
-  </si>
-  <si>
     <t>What science fiction writer wrote the three laws of robotics?</t>
   </si>
   <si>
-    <t>True or false? In computing, keyboards are used as input devices.</t>
-  </si>
-  <si>
     <t>What does the abbreviation WWW stand for?</t>
   </si>
   <si>
     <t>Nano, Shuffle, Classic and Touch are variations of what?</t>
   </si>
   <si>
-    <t>True or false? DNA is an abbreviation for ‘Deoxyribonucleic acid’.</t>
-  </si>
-  <si>
     <t>The Sun</t>
   </si>
   <si>
     <t>Central Processing Unit</t>
   </si>
   <si>
-    <t>False - 1889</t>
-  </si>
-  <si>
     <t>Edwin Hubble</t>
   </si>
   <si>
-    <t>Long</t>
-  </si>
-  <si>
-    <t>Web browsers</t>
-  </si>
-  <si>
-    <t>honda</t>
-  </si>
-  <si>
     <t>Read Only Memory</t>
   </si>
   <si>
-    <t>CD's</t>
-  </si>
-  <si>
     <t>International Business Machines</t>
   </si>
   <si>
@@ -131,15 +83,6 @@
     <t>Wood</t>
   </si>
   <si>
-    <t>Computer power unit</t>
-  </si>
-  <si>
-    <t>central power unit</t>
-  </si>
-  <si>
-    <t>computer processing unix</t>
-  </si>
-  <si>
     <t>Albert einstein</t>
   </si>
   <si>
@@ -149,33 +92,12 @@
     <t>Hubert Hubble</t>
   </si>
   <si>
-    <t>short</t>
-  </si>
-  <si>
-    <t>Internet machines</t>
-  </si>
-  <si>
-    <t>internet</t>
-  </si>
-  <si>
     <t>Ford</t>
   </si>
   <si>
-    <t>Gm</t>
-  </si>
-  <si>
     <t>Toyota</t>
   </si>
   <si>
-    <t>Random order mixer</t>
-  </si>
-  <si>
-    <t>random only memory</t>
-  </si>
-  <si>
-    <t>Read order memory</t>
-  </si>
-  <si>
     <t>Cartridges</t>
   </si>
   <si>
@@ -188,9 +110,6 @@
     <t>Internet Buying Metacorp</t>
   </si>
   <si>
-    <t>International Business Money</t>
-  </si>
-  <si>
     <t>International Banking Machine</t>
   </si>
   <si>
@@ -212,27 +131,12 @@
     <t>J.K. Rowling</t>
   </si>
   <si>
-    <t>World without windows</t>
-  </si>
-  <si>
     <t>Washing Without Windex</t>
   </si>
   <si>
-    <t>Wishing with wells</t>
-  </si>
-  <si>
-    <t>Zune</t>
-  </si>
-  <si>
-    <t>phones</t>
-  </si>
-  <si>
     <t>Along with whom did Bill Gates found Microsoft?</t>
   </si>
   <si>
-    <t>What is the Earth’s primary source of energy?</t>
-  </si>
-  <si>
     <t>QuestionText</t>
   </si>
   <si>
@@ -246,6 +150,162 @@
   </si>
   <si>
     <t>AlternateAnswer3</t>
+  </si>
+  <si>
+    <t>From what source do solar panels generate electricity?</t>
+  </si>
+  <si>
+    <t>In what year did the Apple iPhone first become available?</t>
+  </si>
+  <si>
+    <t>In what year was Nintendo founded?</t>
+  </si>
+  <si>
+    <t>For what reason can humans not see infrared light?</t>
+  </si>
+  <si>
+    <t>Its wavelength is too long.</t>
+  </si>
+  <si>
+    <t>Its wavelength is too short.</t>
+  </si>
+  <si>
+    <t>It isn't bright enough.</t>
+  </si>
+  <si>
+    <t>Its frequency is too high.</t>
+  </si>
+  <si>
+    <t>What company publishes the Firefox web browser?</t>
+  </si>
+  <si>
+    <t>Mozilla</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Which metal is the best electrical conductor?</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Steel</t>
+  </si>
+  <si>
+    <t>Iron</t>
+  </si>
+  <si>
+    <t>Metal doesn't conduct electricity.</t>
+  </si>
+  <si>
+    <t>Honda</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>Upon what scientific principal are nuclear bombs based?</t>
+  </si>
+  <si>
+    <t>Big bomb go boom.</t>
+  </si>
+  <si>
+    <t>Atomic fission</t>
+  </si>
+  <si>
+    <t>Ohm's law</t>
+  </si>
+  <si>
+    <t>Random Order Mixer</t>
+  </si>
+  <si>
+    <t>Radioactive Object Maker</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rational Objective Multiplier</t>
+  </si>
+  <si>
+    <t>What form of digital media did the original PlayStation use for game storage?</t>
+  </si>
+  <si>
+    <t>CDs</t>
+  </si>
+  <si>
+    <t>Papyrus</t>
+  </si>
+  <si>
+    <t>USB stick</t>
+  </si>
+  <si>
+    <t>From what source does the earth get the majority of its energy?</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>What does the company name "IBM" stand for?</t>
+  </si>
+  <si>
+    <t>Internally Bursting Molecule</t>
+  </si>
+  <si>
+    <t>World Without Windows</t>
+  </si>
+  <si>
+    <t>Wishing With Wells</t>
+  </si>
+  <si>
+    <t>Dance moves</t>
+  </si>
+  <si>
+    <t>Microsoft Zune</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Deoxyribonucleic Acid</t>
+  </si>
+  <si>
+    <t>Does Not Apply</t>
+  </si>
+  <si>
+    <t>Do Not Abbreviate</t>
+  </si>
+  <si>
+    <t>Definetely Not an Acronym</t>
+  </si>
+  <si>
+    <t>In biology, what does DNA stand for?</t>
+  </si>
+  <si>
+    <t>The connection is secure.</t>
+  </si>
+  <si>
+    <t>The connection is simple.</t>
+  </si>
+  <si>
+    <t>The browser is confused.</t>
+  </si>
+  <si>
+    <t>What does the "S" at the end of "HTTPS" signify in a web address?</t>
+  </si>
+  <si>
+    <t>The website is saying you're stupid.</t>
+  </si>
+  <si>
+    <t>Computer Power Unifier</t>
+  </si>
+  <si>
+    <t>Certified Professional Undergrad</t>
+  </si>
+  <si>
+    <t>Can't Power Up</t>
   </si>
 </sst>
 </file>
@@ -566,55 +626,55 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="87.42578125" customWidth="1"/>
     <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
         <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <v>2007</v>
@@ -628,257 +688,305 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <v>1889</v>
+      </c>
+      <c r="C5">
+        <v>1928</v>
+      </c>
+      <c r="D5">
+        <v>1946</v>
+      </c>
+      <c r="E5">
+        <v>1983</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
         <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="b">
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="b">
-        <v>1</v>
-      </c>
-      <c r="C11" t="b">
-        <v>0</v>
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
         <v>27</v>
       </c>
-      <c r="C15" t="s">
-        <v>53</v>
-      </c>
       <c r="D15" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
         <v>13</v>
       </c>
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
         <v>14</v>
       </c>
-      <c r="B18" t="b">
-        <v>1</v>
-      </c>
-      <c r="C18" t="b">
-        <v>0</v>
+      <c r="C18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
         <v>15</v>
       </c>
-      <c r="B19" t="s">
-        <v>30</v>
-      </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>83</v>
+      </c>
+      <c r="E20" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" t="b">
-        <v>1</v>
-      </c>
-      <c r="C21" t="b">
-        <v>0</v>
+        <v>89</v>
+      </c>
+      <c r="B21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>